<commit_message>
feat: now checks for valid/invalid url's
This fixes wrong, broken or not valid url.

docs: Updatation for requirements
</commit_message>
<xml_diff>
--- a/excel_reports/19-08-2022.xlsx
+++ b/excel_reports/19-08-2022.xlsx
@@ -477,20 +477,25 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>test_checking[chrome-head]</t>
+          <t>test_checking[chrome]</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>PASSED</t>
+          <t>FAILED</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>5.783368080999935</v>
+        <v>0.03103728900896385</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2022-08-19T14:18:49</t>
+          <t>2022-08-19T14:44:56</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>AssertionError: Please enter a valid URL... http://127.0.0.1:5500/sample.html is not a valid URL.</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">

</xml_diff>

<commit_message>
feat: Dynamic dropdown function added
feat: url check for goto function

refactor: deleted comments from conftest.py

style: added js and css to sample.html

docs: added new example for dynamic dropdown
</commit_message>
<xml_diff>
--- a/excel_reports/19-08-2022.xlsx
+++ b/excel_reports/19-08-2022.xlsx
@@ -482,20 +482,15 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>FAILED</t>
+          <t>PASSED</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0.03103728900896385</v>
+        <v>8.212997483002255</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2022-08-19T14:44:56</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>AssertionError: Please enter a valid URL... http://127.0.0.1:5500/sample.html is not a valid URL.</t>
+          <t>2022-08-19T17:20:39</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">

</xml_diff>

<commit_message>
feat: popup alert feature added
refactor: updated dynamic_dropdown function

docs: added new example for popup alert function
</commit_message>
<xml_diff>
--- a/excel_reports/19-08-2022.xlsx
+++ b/excel_reports/19-08-2022.xlsx
@@ -477,7 +477,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>test_checking[chrome]</t>
+          <t>test_checking[chrome-head]</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -486,11 +486,11 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>8.212997483002255</v>
+        <v>10.11267767900426</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2022-08-19T17:20:39</t>
+          <t>2022-08-19T18:44:16</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">

</xml_diff>